<commit_message>
cucumber normal scene and outline scene
</commit_message>
<xml_diff>
--- a/NAH/data/DataDriven.xlsx
+++ b/NAH/data/DataDriven.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NEXSOFT\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TRAINING\SQA\NAH\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,49 +24,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>Nico</t>
-  </si>
-  <si>
-    <t>Ardy</t>
-  </si>
-  <si>
-    <t>Jakarta</t>
-  </si>
-  <si>
-    <t>Nardi</t>
-  </si>
-  <si>
-    <t>Yoka</t>
-  </si>
-  <si>
-    <t>Bandung</t>
-  </si>
-  <si>
-    <t>Valentino</t>
-  </si>
-  <si>
-    <t>Valko</t>
-  </si>
-  <si>
-    <t>Hera</t>
-  </si>
-  <si>
-    <t>Abyss</t>
-  </si>
-  <si>
-    <t>China</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+  <si>
+    <t>Admin@yourstore.com</t>
+  </si>
+  <si>
+    <t>ADMIN@YOURSTORE.COM</t>
+  </si>
+  <si>
+    <t>ADMIN@yourstore.com</t>
+  </si>
+  <si>
+    <t>admin@yourstore.com</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>admin1</t>
+  </si>
+  <si>
+    <t>admin2</t>
+  </si>
+  <si>
+    <t>admin3</t>
+  </si>
+  <si>
+    <t>admin4</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,13 +97,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -374,83 +385,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>18</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>21</v>
-      </c>
-      <c r="E3">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>19</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A8" r:id="rId4"/>
+    <hyperlink ref="A9" r:id="rId5"/>
+    <hyperlink ref="A5" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>